<commit_message>
Update 17th pe (2007)
</commit_message>
<xml_diff>
--- a/kor2eng.xlsx
+++ b/kor2eng.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/SeungwooKang_1/Documents/GitHub/south-korea-election/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Documents/GitHub/south-korea-election/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338760DC-5EE9-494C-8281-D35994355423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E53337-00B7-8744-8BE2-BD2B15D03B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19080" yWindow="500" windowWidth="19080" windowHeight="21100" xr2:uid="{485E5265-5BD5-BA4D-8DB3-B0C0895E5122}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="516">
   <si>
     <t>종로구</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1809,6 +1809,58 @@
   </si>
   <si>
     <t>Yeoju-gun</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>천안시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cheonan-si</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연기군</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yeongi-gun</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>당진군</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dangjin-gun</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>창원시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Changwon-si</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>고성군</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마산시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>진해시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Masan-si</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jinhae-si</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2173,10 +2225,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7418C56A-0A02-6E49-BE92-F2987AC8A519}">
-  <dimension ref="A1:D256"/>
+  <dimension ref="A1:D262"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="D112" sqref="D112"/>
+    <sheetView tabSelected="1" topLeftCell="A232" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="E241" sqref="E241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -4387,13 +4439,13 @@
         <v>285</v>
       </c>
       <c r="B158" t="s">
-        <v>271</v>
+        <v>503</v>
       </c>
       <c r="C158" t="s">
         <v>386</v>
       </c>
       <c r="D158" t="s">
-        <v>389</v>
+        <v>504</v>
       </c>
     </row>
     <row r="159" spans="1:4">
@@ -4401,13 +4453,13 @@
         <v>285</v>
       </c>
       <c r="B159" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C159" t="s">
         <v>386</v>
       </c>
       <c r="D159" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -4415,13 +4467,13 @@
         <v>285</v>
       </c>
       <c r="B160" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C160" t="s">
         <v>386</v>
       </c>
       <c r="D160" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="161" spans="1:4">
@@ -4429,13 +4481,13 @@
         <v>285</v>
       </c>
       <c r="B161" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C161" t="s">
         <v>386</v>
       </c>
       <c r="D161" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="162" spans="1:4">
@@ -4443,13 +4495,13 @@
         <v>285</v>
       </c>
       <c r="B162" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C162" t="s">
         <v>386</v>
       </c>
       <c r="D162" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="163" spans="1:4">
@@ -4457,13 +4509,13 @@
         <v>285</v>
       </c>
       <c r="B163" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C163" t="s">
         <v>386</v>
       </c>
       <c r="D163" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="164" spans="1:4">
@@ -4471,13 +4523,13 @@
         <v>285</v>
       </c>
       <c r="B164" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C164" t="s">
         <v>386</v>
       </c>
       <c r="D164" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="165" spans="1:4">
@@ -4485,13 +4537,13 @@
         <v>285</v>
       </c>
       <c r="B165" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C165" t="s">
         <v>386</v>
       </c>
       <c r="D165" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="166" spans="1:4">
@@ -4499,13 +4551,13 @@
         <v>285</v>
       </c>
       <c r="B166" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C166" t="s">
         <v>386</v>
       </c>
       <c r="D166" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="167" spans="1:4">
@@ -4513,13 +4565,13 @@
         <v>285</v>
       </c>
       <c r="B167" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C167" t="s">
         <v>386</v>
       </c>
       <c r="D167" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="168" spans="1:4">
@@ -4527,13 +4579,13 @@
         <v>285</v>
       </c>
       <c r="B168" t="s">
-        <v>281</v>
+        <v>507</v>
       </c>
       <c r="C168" t="s">
         <v>386</v>
       </c>
       <c r="D168" t="s">
-        <v>399</v>
+        <v>508</v>
       </c>
     </row>
     <row r="169" spans="1:4">
@@ -4541,13 +4593,13 @@
         <v>285</v>
       </c>
       <c r="B169" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C169" t="s">
         <v>386</v>
       </c>
       <c r="D169" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="170" spans="1:4">
@@ -4555,13 +4607,13 @@
         <v>285</v>
       </c>
       <c r="B170" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C170" t="s">
         <v>386</v>
       </c>
       <c r="D170" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="171" spans="1:4">
@@ -4569,55 +4621,55 @@
         <v>285</v>
       </c>
       <c r="B171" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C171" t="s">
         <v>386</v>
       </c>
       <c r="D171" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="172" spans="1:4">
       <c r="A172" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B172" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C172" t="s">
-        <v>404</v>
+        <v>386</v>
       </c>
       <c r="D172" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="173" spans="1:4">
       <c r="A173" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B173" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C173" t="s">
-        <v>404</v>
+        <v>386</v>
       </c>
       <c r="D173" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="174" spans="1:4">
       <c r="A174" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B174" t="s">
-        <v>289</v>
+        <v>505</v>
       </c>
       <c r="C174" t="s">
-        <v>404</v>
+        <v>386</v>
       </c>
       <c r="D174" t="s">
-        <v>406</v>
+        <v>506</v>
       </c>
     </row>
     <row r="175" spans="1:4">
@@ -4625,13 +4677,13 @@
         <v>286</v>
       </c>
       <c r="B175" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C175" t="s">
         <v>404</v>
       </c>
       <c r="D175" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="176" spans="1:4">
@@ -4639,13 +4691,13 @@
         <v>286</v>
       </c>
       <c r="B176" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C176" t="s">
         <v>404</v>
       </c>
       <c r="D176" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
     <row r="177" spans="1:4">
@@ -4653,13 +4705,13 @@
         <v>286</v>
       </c>
       <c r="B177" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C177" t="s">
         <v>404</v>
       </c>
       <c r="D177" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
     </row>
     <row r="178" spans="1:4">
@@ -4667,13 +4719,13 @@
         <v>286</v>
       </c>
       <c r="B178" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C178" t="s">
         <v>404</v>
       </c>
       <c r="D178" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="179" spans="1:4">
@@ -4681,13 +4733,13 @@
         <v>286</v>
       </c>
       <c r="B179" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C179" t="s">
         <v>404</v>
       </c>
       <c r="D179" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="180" spans="1:4">
@@ -4695,13 +4747,13 @@
         <v>286</v>
       </c>
       <c r="B180" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C180" t="s">
         <v>404</v>
       </c>
       <c r="D180" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="181" spans="1:4">
@@ -4709,13 +4761,13 @@
         <v>286</v>
       </c>
       <c r="B181" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C181" t="s">
         <v>404</v>
       </c>
       <c r="D181" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="182" spans="1:4">
@@ -4723,13 +4775,13 @@
         <v>286</v>
       </c>
       <c r="B182" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C182" t="s">
         <v>404</v>
       </c>
       <c r="D182" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="183" spans="1:4">
@@ -4737,13 +4789,13 @@
         <v>286</v>
       </c>
       <c r="B183" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C183" t="s">
         <v>404</v>
       </c>
       <c r="D183" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="184" spans="1:4">
@@ -4751,13 +4803,13 @@
         <v>286</v>
       </c>
       <c r="B184" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C184" t="s">
         <v>404</v>
       </c>
       <c r="D184" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="185" spans="1:4">
@@ -4765,13 +4817,13 @@
         <v>286</v>
       </c>
       <c r="B185" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C185" t="s">
         <v>404</v>
       </c>
       <c r="D185" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="186" spans="1:4">
@@ -4779,55 +4831,55 @@
         <v>286</v>
       </c>
       <c r="B186" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C186" t="s">
         <v>404</v>
       </c>
       <c r="D186" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="187" spans="1:4">
       <c r="A187" t="s">
-        <v>324</v>
+        <v>286</v>
       </c>
       <c r="B187" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C187" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="D187" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="188" spans="1:4">
       <c r="A188" t="s">
-        <v>324</v>
+        <v>286</v>
       </c>
       <c r="B188" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C188" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="D188" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="189" spans="1:4">
       <c r="A189" t="s">
-        <v>324</v>
+        <v>286</v>
       </c>
       <c r="B189" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C189" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="D189" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="190" spans="1:4">
@@ -4835,13 +4887,13 @@
         <v>324</v>
       </c>
       <c r="B190" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C190" t="s">
         <v>419</v>
       </c>
       <c r="D190" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="191" spans="1:4">
@@ -4849,13 +4901,13 @@
         <v>324</v>
       </c>
       <c r="B191" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C191" t="s">
         <v>419</v>
       </c>
       <c r="D191" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="192" spans="1:4">
@@ -4863,13 +4915,13 @@
         <v>324</v>
       </c>
       <c r="B192" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C192" t="s">
         <v>419</v>
       </c>
       <c r="D192" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="193" spans="1:4">
@@ -4877,13 +4929,13 @@
         <v>324</v>
       </c>
       <c r="B193" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C193" t="s">
         <v>419</v>
       </c>
       <c r="D193" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
     </row>
     <row r="194" spans="1:4">
@@ -4891,13 +4943,13 @@
         <v>324</v>
       </c>
       <c r="B194" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C194" t="s">
         <v>419</v>
       </c>
       <c r="D194" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="195" spans="1:4">
@@ -4905,13 +4957,13 @@
         <v>324</v>
       </c>
       <c r="B195" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C195" t="s">
         <v>419</v>
       </c>
       <c r="D195" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="196" spans="1:4">
@@ -4919,13 +4971,13 @@
         <v>324</v>
       </c>
       <c r="B196" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C196" t="s">
         <v>419</v>
       </c>
       <c r="D196" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="197" spans="1:4">
@@ -4933,13 +4985,13 @@
         <v>324</v>
       </c>
       <c r="B197" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C197" t="s">
         <v>419</v>
       </c>
       <c r="D197" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="198" spans="1:4">
@@ -4947,13 +4999,13 @@
         <v>324</v>
       </c>
       <c r="B198" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C198" t="s">
         <v>419</v>
       </c>
       <c r="D198" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="199" spans="1:4">
@@ -4961,13 +5013,13 @@
         <v>324</v>
       </c>
       <c r="B199" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C199" t="s">
         <v>419</v>
       </c>
       <c r="D199" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
     </row>
     <row r="200" spans="1:4">
@@ -4975,13 +5027,13 @@
         <v>324</v>
       </c>
       <c r="B200" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C200" t="s">
         <v>419</v>
       </c>
       <c r="D200" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
     </row>
     <row r="201" spans="1:4">
@@ -4989,13 +5041,13 @@
         <v>324</v>
       </c>
       <c r="B201" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C201" t="s">
         <v>419</v>
       </c>
       <c r="D201" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="202" spans="1:4">
@@ -5003,13 +5055,13 @@
         <v>324</v>
       </c>
       <c r="B202" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C202" t="s">
         <v>419</v>
       </c>
       <c r="D202" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
     </row>
     <row r="203" spans="1:4">
@@ -5017,13 +5069,13 @@
         <v>324</v>
       </c>
       <c r="B203" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C203" t="s">
         <v>419</v>
       </c>
       <c r="D203" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
     <row r="204" spans="1:4">
@@ -5031,13 +5083,13 @@
         <v>324</v>
       </c>
       <c r="B204" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C204" t="s">
         <v>419</v>
       </c>
       <c r="D204" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="205" spans="1:4">
@@ -5045,13 +5097,13 @@
         <v>324</v>
       </c>
       <c r="B205" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C205" t="s">
         <v>419</v>
       </c>
       <c r="D205" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
     <row r="206" spans="1:4">
@@ -5059,13 +5111,13 @@
         <v>324</v>
       </c>
       <c r="B206" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C206" t="s">
         <v>419</v>
       </c>
       <c r="D206" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
     </row>
     <row r="207" spans="1:4">
@@ -5073,13 +5125,13 @@
         <v>324</v>
       </c>
       <c r="B207" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C207" t="s">
         <v>419</v>
       </c>
       <c r="D207" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="208" spans="1:4">
@@ -5087,55 +5139,55 @@
         <v>324</v>
       </c>
       <c r="B208" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C208" t="s">
         <v>419</v>
       </c>
       <c r="D208" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="209" spans="1:4">
       <c r="A209" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B209" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="C209" t="s">
-        <v>443</v>
+        <v>419</v>
       </c>
       <c r="D209" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="210" spans="1:4">
       <c r="A210" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B210" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="C210" t="s">
-        <v>443</v>
+        <v>419</v>
       </c>
       <c r="D210" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
     </row>
     <row r="211" spans="1:4">
       <c r="A211" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B211" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="C211" t="s">
-        <v>443</v>
+        <v>419</v>
       </c>
       <c r="D211" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
     </row>
     <row r="212" spans="1:4">
@@ -5143,13 +5195,13 @@
         <v>325</v>
       </c>
       <c r="B212" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C212" t="s">
         <v>443</v>
       </c>
       <c r="D212" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
     </row>
     <row r="213" spans="1:4">
@@ -5157,13 +5209,13 @@
         <v>325</v>
       </c>
       <c r="B213" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C213" t="s">
         <v>443</v>
       </c>
       <c r="D213" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="214" spans="1:4">
@@ -5171,13 +5223,13 @@
         <v>325</v>
       </c>
       <c r="B214" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C214" t="s">
         <v>443</v>
       </c>
       <c r="D214" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="215" spans="1:4">
@@ -5185,13 +5237,13 @@
         <v>325</v>
       </c>
       <c r="B215" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C215" t="s">
         <v>443</v>
       </c>
       <c r="D215" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="216" spans="1:4">
@@ -5199,13 +5251,13 @@
         <v>325</v>
       </c>
       <c r="B216" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C216" t="s">
         <v>443</v>
       </c>
       <c r="D216" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="217" spans="1:4">
@@ -5213,13 +5265,13 @@
         <v>325</v>
       </c>
       <c r="B217" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C217" t="s">
         <v>443</v>
       </c>
       <c r="D217" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="218" spans="1:4">
@@ -5227,13 +5279,13 @@
         <v>325</v>
       </c>
       <c r="B218" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C218" t="s">
         <v>443</v>
       </c>
       <c r="D218" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="219" spans="1:4">
@@ -5241,13 +5293,13 @@
         <v>325</v>
       </c>
       <c r="B219" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C219" t="s">
         <v>443</v>
       </c>
       <c r="D219" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="220" spans="1:4">
@@ -5255,13 +5307,13 @@
         <v>325</v>
       </c>
       <c r="B220" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C220" t="s">
         <v>443</v>
       </c>
       <c r="D220" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="221" spans="1:4">
@@ -5269,13 +5321,13 @@
         <v>325</v>
       </c>
       <c r="B221" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C221" t="s">
         <v>443</v>
       </c>
       <c r="D221" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="222" spans="1:4">
@@ -5283,13 +5335,13 @@
         <v>325</v>
       </c>
       <c r="B222" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C222" t="s">
         <v>443</v>
       </c>
       <c r="D222" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="223" spans="1:4">
@@ -5297,13 +5349,13 @@
         <v>325</v>
       </c>
       <c r="B223" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C223" t="s">
         <v>443</v>
       </c>
       <c r="D223" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="224" spans="1:4">
@@ -5311,13 +5363,13 @@
         <v>325</v>
       </c>
       <c r="B224" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C224" t="s">
         <v>443</v>
       </c>
       <c r="D224" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
     </row>
     <row r="225" spans="1:4">
@@ -5325,13 +5377,13 @@
         <v>325</v>
       </c>
       <c r="B225" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C225" t="s">
         <v>443</v>
       </c>
       <c r="D225" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="226" spans="1:4">
@@ -5339,13 +5391,13 @@
         <v>325</v>
       </c>
       <c r="B226" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C226" t="s">
         <v>443</v>
       </c>
       <c r="D226" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
     </row>
     <row r="227" spans="1:4">
@@ -5353,13 +5405,13 @@
         <v>325</v>
       </c>
       <c r="B227" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C227" t="s">
         <v>443</v>
       </c>
       <c r="D227" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="228" spans="1:4">
@@ -5367,13 +5419,13 @@
         <v>325</v>
       </c>
       <c r="B228" t="s">
-        <v>462</v>
+        <v>342</v>
       </c>
       <c r="C228" t="s">
         <v>443</v>
       </c>
       <c r="D228" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
     </row>
     <row r="229" spans="1:4">
@@ -5381,13 +5433,13 @@
         <v>325</v>
       </c>
       <c r="B229" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C229" t="s">
         <v>443</v>
       </c>
       <c r="D229" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
     </row>
     <row r="230" spans="1:4">
@@ -5395,13 +5447,13 @@
         <v>325</v>
       </c>
       <c r="B230" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C230" t="s">
         <v>443</v>
       </c>
       <c r="D230" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
     </row>
     <row r="231" spans="1:4">
@@ -5409,13 +5461,13 @@
         <v>325</v>
       </c>
       <c r="B231" t="s">
-        <v>347</v>
+        <v>462</v>
       </c>
       <c r="C231" t="s">
         <v>443</v>
       </c>
       <c r="D231" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
     </row>
     <row r="232" spans="1:4">
@@ -5423,55 +5475,55 @@
         <v>325</v>
       </c>
       <c r="B232" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C232" t="s">
         <v>443</v>
       </c>
       <c r="D232" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="233" spans="1:4">
       <c r="A233" t="s">
-        <v>349</v>
+        <v>325</v>
       </c>
       <c r="B233" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C233" t="s">
-        <v>469</v>
+        <v>443</v>
       </c>
       <c r="D233" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
     <row r="234" spans="1:4">
       <c r="A234" t="s">
-        <v>349</v>
+        <v>325</v>
       </c>
       <c r="B234" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="C234" t="s">
-        <v>469</v>
+        <v>443</v>
       </c>
       <c r="D234" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
     </row>
     <row r="235" spans="1:4">
       <c r="A235" t="s">
-        <v>349</v>
+        <v>325</v>
       </c>
       <c r="B235" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C235" t="s">
-        <v>469</v>
+        <v>443</v>
       </c>
       <c r="D235" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
     </row>
     <row r="236" spans="1:4">
@@ -5479,13 +5531,13 @@
         <v>349</v>
       </c>
       <c r="B236" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C236" t="s">
         <v>469</v>
       </c>
       <c r="D236" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
     </row>
     <row r="237" spans="1:4">
@@ -5493,13 +5545,13 @@
         <v>349</v>
       </c>
       <c r="B237" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C237" t="s">
         <v>469</v>
       </c>
       <c r="D237" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
     </row>
     <row r="238" spans="1:4">
@@ -5507,13 +5559,13 @@
         <v>349</v>
       </c>
       <c r="B238" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C238" t="s">
         <v>469</v>
       </c>
       <c r="D238" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="239" spans="1:4">
@@ -5521,13 +5573,13 @@
         <v>349</v>
       </c>
       <c r="B239" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C239" t="s">
         <v>469</v>
       </c>
       <c r="D239" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="240" spans="1:4">
@@ -5535,13 +5587,13 @@
         <v>349</v>
       </c>
       <c r="B240" t="s">
-        <v>159</v>
+        <v>354</v>
       </c>
       <c r="C240" t="s">
         <v>469</v>
       </c>
       <c r="D240" t="s">
-        <v>241</v>
+        <v>473</v>
       </c>
     </row>
     <row r="241" spans="1:4">
@@ -5549,13 +5601,13 @@
         <v>349</v>
       </c>
       <c r="B241" t="s">
-        <v>357</v>
+        <v>509</v>
       </c>
       <c r="C241" t="s">
         <v>469</v>
       </c>
       <c r="D241" t="s">
-        <v>476</v>
+        <v>510</v>
       </c>
     </row>
     <row r="242" spans="1:4">
@@ -5563,13 +5615,13 @@
         <v>349</v>
       </c>
       <c r="B242" t="s">
-        <v>358</v>
+        <v>512</v>
       </c>
       <c r="C242" t="s">
         <v>469</v>
       </c>
       <c r="D242" t="s">
-        <v>477</v>
+        <v>514</v>
       </c>
     </row>
     <row r="243" spans="1:4">
@@ -5577,13 +5629,13 @@
         <v>349</v>
       </c>
       <c r="B243" t="s">
-        <v>359</v>
+        <v>513</v>
       </c>
       <c r="C243" t="s">
         <v>469</v>
       </c>
       <c r="D243" t="s">
-        <v>478</v>
+        <v>515</v>
       </c>
     </row>
     <row r="244" spans="1:4">
@@ -5591,13 +5643,13 @@
         <v>349</v>
       </c>
       <c r="B244" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="C244" t="s">
         <v>469</v>
       </c>
       <c r="D244" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
     </row>
     <row r="245" spans="1:4">
@@ -5605,13 +5657,13 @@
         <v>349</v>
       </c>
       <c r="B245" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="C245" t="s">
         <v>469</v>
       </c>
       <c r="D245" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
     </row>
     <row r="246" spans="1:4">
@@ -5619,13 +5671,13 @@
         <v>349</v>
       </c>
       <c r="B246" t="s">
-        <v>362</v>
+        <v>511</v>
       </c>
       <c r="C246" t="s">
         <v>469</v>
       </c>
       <c r="D246" t="s">
-        <v>481</v>
+        <v>241</v>
       </c>
     </row>
     <row r="247" spans="1:4">
@@ -5633,13 +5685,13 @@
         <v>349</v>
       </c>
       <c r="B247" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="C247" t="s">
         <v>469</v>
       </c>
       <c r="D247" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
     </row>
     <row r="248" spans="1:4">
@@ -5647,13 +5699,13 @@
         <v>349</v>
       </c>
       <c r="B248" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="C248" t="s">
         <v>469</v>
       </c>
       <c r="D248" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
     </row>
     <row r="249" spans="1:4">
@@ -5661,13 +5713,13 @@
         <v>349</v>
       </c>
       <c r="B249" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="C249" t="s">
         <v>469</v>
       </c>
       <c r="D249" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
     </row>
     <row r="250" spans="1:4">
@@ -5675,13 +5727,13 @@
         <v>349</v>
       </c>
       <c r="B250" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="C250" t="s">
         <v>469</v>
       </c>
       <c r="D250" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
     </row>
     <row r="251" spans="1:4">
@@ -5689,13 +5741,13 @@
         <v>349</v>
       </c>
       <c r="B251" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="C251" t="s">
         <v>469</v>
       </c>
       <c r="D251" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
     </row>
     <row r="252" spans="1:4">
@@ -5703,13 +5755,13 @@
         <v>349</v>
       </c>
       <c r="B252" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="C252" t="s">
         <v>469</v>
       </c>
       <c r="D252" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
     </row>
     <row r="253" spans="1:4">
@@ -5717,13 +5769,13 @@
         <v>349</v>
       </c>
       <c r="B253" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="C253" t="s">
         <v>469</v>
       </c>
       <c r="D253" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
     </row>
     <row r="254" spans="1:4">
@@ -5731,40 +5783,124 @@
         <v>349</v>
       </c>
       <c r="B254" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="C254" t="s">
         <v>469</v>
       </c>
       <c r="D254" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
     </row>
     <row r="255" spans="1:4">
       <c r="A255" t="s">
-        <v>371</v>
+        <v>349</v>
       </c>
       <c r="B255" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="C255" t="s">
-        <v>490</v>
+        <v>469</v>
       </c>
       <c r="D255" t="s">
-        <v>491</v>
+        <v>484</v>
       </c>
     </row>
     <row r="256" spans="1:4">
       <c r="A256" t="s">
+        <v>349</v>
+      </c>
+      <c r="B256" t="s">
+        <v>366</v>
+      </c>
+      <c r="C256" t="s">
+        <v>469</v>
+      </c>
+      <c r="D256" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4">
+      <c r="A257" t="s">
+        <v>349</v>
+      </c>
+      <c r="B257" t="s">
+        <v>367</v>
+      </c>
+      <c r="C257" t="s">
+        <v>469</v>
+      </c>
+      <c r="D257" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4">
+      <c r="A258" t="s">
+        <v>349</v>
+      </c>
+      <c r="B258" t="s">
+        <v>368</v>
+      </c>
+      <c r="C258" t="s">
+        <v>469</v>
+      </c>
+      <c r="D258" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4">
+      <c r="A259" t="s">
+        <v>349</v>
+      </c>
+      <c r="B259" t="s">
+        <v>369</v>
+      </c>
+      <c r="C259" t="s">
+        <v>469</v>
+      </c>
+      <c r="D259" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4">
+      <c r="A260" t="s">
+        <v>349</v>
+      </c>
+      <c r="B260" t="s">
+        <v>370</v>
+      </c>
+      <c r="C260" t="s">
+        <v>469</v>
+      </c>
+      <c r="D260" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4">
+      <c r="A261" t="s">
         <v>371</v>
       </c>
-      <c r="B256" t="s">
+      <c r="B261" t="s">
+        <v>372</v>
+      </c>
+      <c r="C261" t="s">
+        <v>490</v>
+      </c>
+      <c r="D261" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4">
+      <c r="A262" t="s">
+        <v>371</v>
+      </c>
+      <c r="B262" t="s">
         <v>373</v>
       </c>
-      <c r="C256" t="s">
+      <c r="C262" t="s">
         <v>490</v>
       </c>
-      <c r="D256" t="s">
+      <c r="D262" t="s">
         <v>492</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update 16th pe (2002)
</commit_message>
<xml_diff>
--- a/kor2eng.xlsx
+++ b/kor2eng.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Documents/GitHub/south-korea-election/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E53337-00B7-8744-8BE2-BD2B15D03B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A7F256-D151-7946-BE22-DEB12624704A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19080" yWindow="500" windowWidth="19080" windowHeight="21100" xr2:uid="{485E5265-5BD5-BA4D-8DB3-B0C0895E5122}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="528">
   <si>
     <t>종로구</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1861,6 +1861,54 @@
   </si>
   <si>
     <t>Jinhae-si</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>양주군</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yangju-gun</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>고양시일산구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ilsan-gu, Goyang-si</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>용인시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yongin-si</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>포천군</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pocheon-gun</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>북제주군</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>남제주군</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bukjeju-gun</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Namjeju-gun</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2225,10 +2273,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7418C56A-0A02-6E49-BE92-F2987AC8A519}">
-  <dimension ref="A1:D262"/>
+  <dimension ref="A1:D268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A232" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="E241" sqref="E241"/>
+    <sheetView tabSelected="1" topLeftCell="A255" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="D269" sqref="D269"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -3543,13 +3591,13 @@
         <v>150</v>
       </c>
       <c r="B94" t="s">
-        <v>122</v>
+        <v>516</v>
       </c>
       <c r="C94" t="s">
         <v>190</v>
       </c>
       <c r="D94" t="s">
-        <v>204</v>
+        <v>517</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -3557,13 +3605,13 @@
         <v>150</v>
       </c>
       <c r="B95" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C95" t="s">
         <v>190</v>
       </c>
       <c r="D95" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -3571,13 +3619,13 @@
         <v>150</v>
       </c>
       <c r="B96" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C96" t="s">
         <v>190</v>
       </c>
       <c r="D96" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -3585,13 +3633,13 @@
         <v>150</v>
       </c>
       <c r="B97" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C97" t="s">
         <v>190</v>
       </c>
       <c r="D97" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -3599,13 +3647,13 @@
         <v>150</v>
       </c>
       <c r="B98" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C98" t="s">
         <v>190</v>
       </c>
       <c r="D98" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -3613,13 +3661,13 @@
         <v>150</v>
       </c>
       <c r="B99" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C99" t="s">
         <v>190</v>
       </c>
       <c r="D99" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -3627,13 +3675,13 @@
         <v>150</v>
       </c>
       <c r="B100" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C100" t="s">
         <v>190</v>
       </c>
       <c r="D100" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -3641,13 +3689,13 @@
         <v>150</v>
       </c>
       <c r="B101" t="s">
-        <v>129</v>
+        <v>518</v>
       </c>
       <c r="C101" t="s">
         <v>190</v>
       </c>
       <c r="D101" t="s">
-        <v>211</v>
+        <v>519</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -3655,13 +3703,13 @@
         <v>150</v>
       </c>
       <c r="B102" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C102" t="s">
         <v>190</v>
       </c>
       <c r="D102" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -3669,13 +3717,13 @@
         <v>150</v>
       </c>
       <c r="B103" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C103" t="s">
         <v>190</v>
       </c>
       <c r="D103" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -3683,13 +3731,13 @@
         <v>150</v>
       </c>
       <c r="B104" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C104" t="s">
         <v>190</v>
       </c>
       <c r="D104" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -3697,13 +3745,13 @@
         <v>150</v>
       </c>
       <c r="B105" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C105" t="s">
         <v>190</v>
       </c>
       <c r="D105" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -3711,13 +3759,13 @@
         <v>150</v>
       </c>
       <c r="B106" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C106" t="s">
         <v>190</v>
       </c>
       <c r="D106" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -3725,13 +3773,13 @@
         <v>150</v>
       </c>
       <c r="B107" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C107" t="s">
         <v>190</v>
       </c>
       <c r="D107" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -3739,13 +3787,13 @@
         <v>150</v>
       </c>
       <c r="B108" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C108" t="s">
         <v>190</v>
       </c>
       <c r="D108" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -3753,13 +3801,13 @@
         <v>150</v>
       </c>
       <c r="B109" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C109" t="s">
         <v>190</v>
       </c>
       <c r="D109" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -3767,13 +3815,13 @@
         <v>150</v>
       </c>
       <c r="B110" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C110" t="s">
         <v>190</v>
       </c>
       <c r="D110" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -3781,13 +3829,13 @@
         <v>150</v>
       </c>
       <c r="B111" t="s">
-        <v>501</v>
+        <v>137</v>
       </c>
       <c r="C111" t="s">
         <v>190</v>
       </c>
       <c r="D111" t="s">
-        <v>502</v>
+        <v>219</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -3795,13 +3843,13 @@
         <v>150</v>
       </c>
       <c r="B112" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C112" t="s">
         <v>190</v>
       </c>
       <c r="D112" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -3809,13 +3857,13 @@
         <v>150</v>
       </c>
       <c r="B113" t="s">
-        <v>140</v>
+        <v>501</v>
       </c>
       <c r="C113" t="s">
         <v>190</v>
       </c>
       <c r="D113" t="s">
-        <v>222</v>
+        <v>502</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -3823,13 +3871,13 @@
         <v>150</v>
       </c>
       <c r="B114" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C114" t="s">
         <v>190</v>
       </c>
       <c r="D114" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -3837,13 +3885,13 @@
         <v>150</v>
       </c>
       <c r="B115" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C115" t="s">
         <v>190</v>
       </c>
       <c r="D115" t="s">
-        <v>239</v>
+        <v>222</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -3851,13 +3899,13 @@
         <v>150</v>
       </c>
       <c r="B116" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C116" t="s">
         <v>190</v>
       </c>
       <c r="D116" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -3865,13 +3913,13 @@
         <v>150</v>
       </c>
       <c r="B117" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C117" t="s">
         <v>190</v>
       </c>
       <c r="D117" t="s">
-        <v>225</v>
+        <v>239</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -3879,13 +3927,13 @@
         <v>150</v>
       </c>
       <c r="B118" t="s">
-        <v>145</v>
+        <v>520</v>
       </c>
       <c r="C118" t="s">
         <v>190</v>
       </c>
       <c r="D118" t="s">
-        <v>226</v>
+        <v>521</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -3893,13 +3941,13 @@
         <v>150</v>
       </c>
       <c r="B119" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C119" t="s">
         <v>190</v>
       </c>
       <c r="D119" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -3907,13 +3955,13 @@
         <v>150</v>
       </c>
       <c r="B120" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C120" t="s">
         <v>190</v>
       </c>
       <c r="D120" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -3921,13 +3969,13 @@
         <v>150</v>
       </c>
       <c r="B121" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C121" t="s">
         <v>190</v>
       </c>
       <c r="D121" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -3935,69 +3983,69 @@
         <v>150</v>
       </c>
       <c r="B122" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C122" t="s">
         <v>190</v>
       </c>
       <c r="D122" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="123" spans="1:4">
       <c r="A123" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="B123" t="s">
-        <v>151</v>
+        <v>522</v>
       </c>
       <c r="C123" t="s">
-        <v>231</v>
+        <v>190</v>
       </c>
       <c r="D123" t="s">
-        <v>232</v>
+        <v>523</v>
       </c>
     </row>
     <row r="124" spans="1:4">
       <c r="A124" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="B124" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C124" t="s">
-        <v>231</v>
+        <v>190</v>
       </c>
       <c r="D124" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="125" spans="1:4">
       <c r="A125" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="B125" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C125" t="s">
-        <v>231</v>
+        <v>190</v>
       </c>
       <c r="D125" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="126" spans="1:4">
       <c r="A126" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="B126" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C126" t="s">
-        <v>231</v>
+        <v>190</v>
       </c>
       <c r="D126" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -4005,13 +4053,13 @@
         <v>169</v>
       </c>
       <c r="B127" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C127" t="s">
         <v>231</v>
       </c>
       <c r="D127" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -4019,13 +4067,13 @@
         <v>169</v>
       </c>
       <c r="B128" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C128" t="s">
         <v>231</v>
       </c>
       <c r="D128" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -4033,13 +4081,13 @@
         <v>169</v>
       </c>
       <c r="B129" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C129" t="s">
         <v>231</v>
       </c>
       <c r="D129" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -4047,13 +4095,13 @@
         <v>169</v>
       </c>
       <c r="B130" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C130" t="s">
         <v>231</v>
       </c>
       <c r="D130" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -4061,13 +4109,13 @@
         <v>169</v>
       </c>
       <c r="B131" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C131" t="s">
         <v>231</v>
       </c>
       <c r="D131" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -4075,13 +4123,13 @@
         <v>169</v>
       </c>
       <c r="B132" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C132" t="s">
         <v>231</v>
       </c>
       <c r="D132" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -4089,13 +4137,13 @@
         <v>169</v>
       </c>
       <c r="B133" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C133" t="s">
         <v>231</v>
       </c>
       <c r="D133" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -4103,13 +4151,13 @@
         <v>169</v>
       </c>
       <c r="B134" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C134" t="s">
         <v>231</v>
       </c>
       <c r="D134" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -4117,13 +4165,13 @@
         <v>169</v>
       </c>
       <c r="B135" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C135" t="s">
         <v>231</v>
       </c>
       <c r="D135" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -4131,13 +4179,13 @@
         <v>169</v>
       </c>
       <c r="B136" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C136" t="s">
         <v>231</v>
       </c>
       <c r="D136" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -4145,13 +4193,13 @@
         <v>169</v>
       </c>
       <c r="B137" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C137" t="s">
         <v>231</v>
       </c>
       <c r="D137" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -4159,13 +4207,13 @@
         <v>169</v>
       </c>
       <c r="B138" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C138" t="s">
         <v>231</v>
       </c>
       <c r="D138" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -4173,13 +4221,13 @@
         <v>169</v>
       </c>
       <c r="B139" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C139" t="s">
         <v>231</v>
       </c>
       <c r="D139" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -4187,69 +4235,69 @@
         <v>169</v>
       </c>
       <c r="B140" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C140" t="s">
         <v>231</v>
       </c>
       <c r="D140" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="141" spans="1:4">
       <c r="A141" t="s">
-        <v>265</v>
+        <v>169</v>
       </c>
       <c r="B141" t="s">
-        <v>251</v>
+        <v>165</v>
       </c>
       <c r="C141" t="s">
-        <v>266</v>
+        <v>231</v>
       </c>
       <c r="D141" t="s">
-        <v>267</v>
+        <v>247</v>
       </c>
     </row>
     <row r="142" spans="1:4">
       <c r="A142" t="s">
-        <v>265</v>
+        <v>169</v>
       </c>
       <c r="B142" t="s">
-        <v>252</v>
+        <v>166</v>
       </c>
       <c r="C142" t="s">
-        <v>266</v>
+        <v>231</v>
       </c>
       <c r="D142" t="s">
-        <v>268</v>
+        <v>248</v>
       </c>
     </row>
     <row r="143" spans="1:4">
       <c r="A143" t="s">
-        <v>265</v>
+        <v>169</v>
       </c>
       <c r="B143" t="s">
-        <v>253</v>
+        <v>167</v>
       </c>
       <c r="C143" t="s">
-        <v>266</v>
+        <v>231</v>
       </c>
       <c r="D143" t="s">
-        <v>374</v>
+        <v>249</v>
       </c>
     </row>
     <row r="144" spans="1:4">
       <c r="A144" t="s">
-        <v>265</v>
+        <v>169</v>
       </c>
       <c r="B144" t="s">
-        <v>254</v>
+        <v>168</v>
       </c>
       <c r="C144" t="s">
-        <v>266</v>
+        <v>231</v>
       </c>
       <c r="D144" t="s">
-        <v>375</v>
+        <v>250</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -4257,13 +4305,13 @@
         <v>265</v>
       </c>
       <c r="B145" t="s">
-        <v>493</v>
+        <v>251</v>
       </c>
       <c r="C145" t="s">
         <v>266</v>
       </c>
       <c r="D145" t="s">
-        <v>494</v>
+        <v>267</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -4271,13 +4319,13 @@
         <v>265</v>
       </c>
       <c r="B146" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C146" t="s">
         <v>266</v>
       </c>
       <c r="D146" t="s">
-        <v>376</v>
+        <v>268</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -4285,13 +4333,13 @@
         <v>265</v>
       </c>
       <c r="B147" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C147" t="s">
         <v>266</v>
       </c>
       <c r="D147" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="148" spans="1:4">
@@ -4299,13 +4347,13 @@
         <v>265</v>
       </c>
       <c r="B148" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C148" t="s">
         <v>266</v>
       </c>
       <c r="D148" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="149" spans="1:4">
@@ -4313,13 +4361,13 @@
         <v>265</v>
       </c>
       <c r="B149" t="s">
-        <v>258</v>
+        <v>493</v>
       </c>
       <c r="C149" t="s">
         <v>266</v>
       </c>
       <c r="D149" t="s">
-        <v>379</v>
+        <v>494</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -4327,13 +4375,13 @@
         <v>265</v>
       </c>
       <c r="B150" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C150" t="s">
         <v>266</v>
       </c>
       <c r="D150" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -4341,13 +4389,13 @@
         <v>265</v>
       </c>
       <c r="B151" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C151" t="s">
         <v>266</v>
       </c>
       <c r="D151" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -4355,13 +4403,13 @@
         <v>265</v>
       </c>
       <c r="B152" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C152" t="s">
         <v>266</v>
       </c>
       <c r="D152" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="153" spans="1:4">
@@ -4369,13 +4417,13 @@
         <v>265</v>
       </c>
       <c r="B153" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C153" t="s">
         <v>266</v>
       </c>
       <c r="D153" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="154" spans="1:4">
@@ -4383,13 +4431,13 @@
         <v>265</v>
       </c>
       <c r="B154" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C154" t="s">
         <v>266</v>
       </c>
       <c r="D154" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="155" spans="1:4">
@@ -4397,69 +4445,69 @@
         <v>265</v>
       </c>
       <c r="B155" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C155" t="s">
         <v>266</v>
       </c>
       <c r="D155" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="156" spans="1:4">
       <c r="A156" t="s">
-        <v>285</v>
+        <v>265</v>
       </c>
       <c r="B156" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="C156" t="s">
-        <v>386</v>
+        <v>266</v>
       </c>
       <c r="D156" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
     </row>
     <row r="157" spans="1:4">
       <c r="A157" t="s">
-        <v>285</v>
+        <v>265</v>
       </c>
       <c r="B157" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="C157" t="s">
-        <v>386</v>
+        <v>266</v>
       </c>
       <c r="D157" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
     </row>
     <row r="158" spans="1:4">
       <c r="A158" t="s">
-        <v>285</v>
+        <v>265</v>
       </c>
       <c r="B158" t="s">
-        <v>503</v>
+        <v>263</v>
       </c>
       <c r="C158" t="s">
-        <v>386</v>
+        <v>266</v>
       </c>
       <c r="D158" t="s">
-        <v>504</v>
+        <v>384</v>
       </c>
     </row>
     <row r="159" spans="1:4">
       <c r="A159" t="s">
-        <v>285</v>
+        <v>265</v>
       </c>
       <c r="B159" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="C159" t="s">
-        <v>386</v>
+        <v>266</v>
       </c>
       <c r="D159" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -4467,13 +4515,13 @@
         <v>285</v>
       </c>
       <c r="B160" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C160" t="s">
         <v>386</v>
       </c>
       <c r="D160" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="161" spans="1:4">
@@ -4481,13 +4529,13 @@
         <v>285</v>
       </c>
       <c r="B161" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C161" t="s">
         <v>386</v>
       </c>
       <c r="D161" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="162" spans="1:4">
@@ -4495,13 +4543,13 @@
         <v>285</v>
       </c>
       <c r="B162" t="s">
-        <v>274</v>
+        <v>503</v>
       </c>
       <c r="C162" t="s">
         <v>386</v>
       </c>
       <c r="D162" t="s">
-        <v>392</v>
+        <v>504</v>
       </c>
     </row>
     <row r="163" spans="1:4">
@@ -4509,13 +4557,13 @@
         <v>285</v>
       </c>
       <c r="B163" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C163" t="s">
         <v>386</v>
       </c>
       <c r="D163" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="164" spans="1:4">
@@ -4523,13 +4571,13 @@
         <v>285</v>
       </c>
       <c r="B164" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C164" t="s">
         <v>386</v>
       </c>
       <c r="D164" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="165" spans="1:4">
@@ -4537,13 +4585,13 @@
         <v>285</v>
       </c>
       <c r="B165" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="C165" t="s">
         <v>386</v>
       </c>
       <c r="D165" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="166" spans="1:4">
@@ -4551,13 +4599,13 @@
         <v>285</v>
       </c>
       <c r="B166" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C166" t="s">
         <v>386</v>
       </c>
       <c r="D166" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="167" spans="1:4">
@@ -4565,13 +4613,13 @@
         <v>285</v>
       </c>
       <c r="B167" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C167" t="s">
         <v>386</v>
       </c>
       <c r="D167" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="168" spans="1:4">
@@ -4579,13 +4627,13 @@
         <v>285</v>
       </c>
       <c r="B168" t="s">
-        <v>507</v>
+        <v>276</v>
       </c>
       <c r="C168" t="s">
         <v>386</v>
       </c>
       <c r="D168" t="s">
-        <v>508</v>
+        <v>394</v>
       </c>
     </row>
     <row r="169" spans="1:4">
@@ -4593,13 +4641,13 @@
         <v>285</v>
       </c>
       <c r="B169" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C169" t="s">
         <v>386</v>
       </c>
       <c r="D169" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="170" spans="1:4">
@@ -4607,13 +4655,13 @@
         <v>285</v>
       </c>
       <c r="B170" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C170" t="s">
         <v>386</v>
       </c>
       <c r="D170" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="171" spans="1:4">
@@ -4621,13 +4669,13 @@
         <v>285</v>
       </c>
       <c r="B171" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C171" t="s">
         <v>386</v>
       </c>
       <c r="D171" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="172" spans="1:4">
@@ -4635,13 +4683,13 @@
         <v>285</v>
       </c>
       <c r="B172" t="s">
-        <v>283</v>
+        <v>507</v>
       </c>
       <c r="C172" t="s">
         <v>386</v>
       </c>
       <c r="D172" t="s">
-        <v>401</v>
+        <v>508</v>
       </c>
     </row>
     <row r="173" spans="1:4">
@@ -4649,13 +4697,13 @@
         <v>285</v>
       </c>
       <c r="B173" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C173" t="s">
         <v>386</v>
       </c>
       <c r="D173" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="174" spans="1:4">
@@ -4663,69 +4711,69 @@
         <v>285</v>
       </c>
       <c r="B174" t="s">
-        <v>505</v>
+        <v>281</v>
       </c>
       <c r="C174" t="s">
         <v>386</v>
       </c>
       <c r="D174" t="s">
-        <v>506</v>
+        <v>399</v>
       </c>
     </row>
     <row r="175" spans="1:4">
       <c r="A175" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B175" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="C175" t="s">
-        <v>404</v>
+        <v>386</v>
       </c>
       <c r="D175" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
     </row>
     <row r="176" spans="1:4">
       <c r="A176" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B176" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="C176" t="s">
-        <v>404</v>
+        <v>386</v>
       </c>
       <c r="D176" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="177" spans="1:4">
       <c r="A177" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B177" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="C177" t="s">
-        <v>404</v>
+        <v>386</v>
       </c>
       <c r="D177" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="178" spans="1:4">
       <c r="A178" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B178" t="s">
-        <v>290</v>
+        <v>505</v>
       </c>
       <c r="C178" t="s">
-        <v>404</v>
+        <v>386</v>
       </c>
       <c r="D178" t="s">
-        <v>407</v>
+        <v>506</v>
       </c>
     </row>
     <row r="179" spans="1:4">
@@ -4733,13 +4781,13 @@
         <v>286</v>
       </c>
       <c r="B179" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C179" t="s">
         <v>404</v>
       </c>
       <c r="D179" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
     </row>
     <row r="180" spans="1:4">
@@ -4747,13 +4795,13 @@
         <v>286</v>
       </c>
       <c r="B180" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="C180" t="s">
         <v>404</v>
       </c>
       <c r="D180" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="181" spans="1:4">
@@ -4761,13 +4809,13 @@
         <v>286</v>
       </c>
       <c r="B181" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C181" t="s">
         <v>404</v>
       </c>
       <c r="D181" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
     </row>
     <row r="182" spans="1:4">
@@ -4775,13 +4823,13 @@
         <v>286</v>
       </c>
       <c r="B182" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C182" t="s">
         <v>404</v>
       </c>
       <c r="D182" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="183" spans="1:4">
@@ -4789,13 +4837,13 @@
         <v>286</v>
       </c>
       <c r="B183" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C183" t="s">
         <v>404</v>
       </c>
       <c r="D183" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
     </row>
     <row r="184" spans="1:4">
@@ -4803,13 +4851,13 @@
         <v>286</v>
       </c>
       <c r="B184" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C184" t="s">
         <v>404</v>
       </c>
       <c r="D184" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="185" spans="1:4">
@@ -4817,13 +4865,13 @@
         <v>286</v>
       </c>
       <c r="B185" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C185" t="s">
         <v>404</v>
       </c>
       <c r="D185" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="186" spans="1:4">
@@ -4831,13 +4879,13 @@
         <v>286</v>
       </c>
       <c r="B186" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C186" t="s">
         <v>404</v>
       </c>
       <c r="D186" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
     </row>
     <row r="187" spans="1:4">
@@ -4845,13 +4893,13 @@
         <v>286</v>
       </c>
       <c r="B187" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C187" t="s">
         <v>404</v>
       </c>
       <c r="D187" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
     </row>
     <row r="188" spans="1:4">
@@ -4859,13 +4907,13 @@
         <v>286</v>
       </c>
       <c r="B188" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C188" t="s">
         <v>404</v>
       </c>
       <c r="D188" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="189" spans="1:4">
@@ -4873,69 +4921,69 @@
         <v>286</v>
       </c>
       <c r="B189" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C189" t="s">
         <v>404</v>
       </c>
       <c r="D189" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="190" spans="1:4">
       <c r="A190" t="s">
-        <v>324</v>
+        <v>286</v>
       </c>
       <c r="B190" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C190" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="D190" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
     </row>
     <row r="191" spans="1:4">
       <c r="A191" t="s">
-        <v>324</v>
+        <v>286</v>
       </c>
       <c r="B191" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="C191" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="D191" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
     </row>
     <row r="192" spans="1:4">
       <c r="A192" t="s">
-        <v>324</v>
+        <v>286</v>
       </c>
       <c r="B192" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C192" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="D192" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
     </row>
     <row r="193" spans="1:4">
       <c r="A193" t="s">
-        <v>324</v>
+        <v>286</v>
       </c>
       <c r="B193" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C193" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="D193" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
     </row>
     <row r="194" spans="1:4">
@@ -4943,13 +4991,13 @@
         <v>324</v>
       </c>
       <c r="B194" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C194" t="s">
         <v>419</v>
       </c>
       <c r="D194" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="195" spans="1:4">
@@ -4957,13 +5005,13 @@
         <v>324</v>
       </c>
       <c r="B195" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="C195" t="s">
         <v>419</v>
       </c>
       <c r="D195" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="196" spans="1:4">
@@ -4971,13 +5019,13 @@
         <v>324</v>
       </c>
       <c r="B196" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="C196" t="s">
         <v>419</v>
       </c>
       <c r="D196" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="197" spans="1:4">
@@ -4985,13 +5033,13 @@
         <v>324</v>
       </c>
       <c r="B197" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C197" t="s">
         <v>419</v>
       </c>
       <c r="D197" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="198" spans="1:4">
@@ -4999,13 +5047,13 @@
         <v>324</v>
       </c>
       <c r="B198" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="C198" t="s">
         <v>419</v>
       </c>
       <c r="D198" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="199" spans="1:4">
@@ -5013,13 +5061,13 @@
         <v>324</v>
       </c>
       <c r="B199" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="C199" t="s">
         <v>419</v>
       </c>
       <c r="D199" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="200" spans="1:4">
@@ -5027,13 +5075,13 @@
         <v>324</v>
       </c>
       <c r="B200" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C200" t="s">
         <v>419</v>
       </c>
       <c r="D200" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="201" spans="1:4">
@@ -5041,13 +5089,13 @@
         <v>324</v>
       </c>
       <c r="B201" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C201" t="s">
         <v>419</v>
       </c>
       <c r="D201" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="202" spans="1:4">
@@ -5055,13 +5103,13 @@
         <v>324</v>
       </c>
       <c r="B202" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C202" t="s">
         <v>419</v>
       </c>
       <c r="D202" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="203" spans="1:4">
@@ -5069,13 +5117,13 @@
         <v>324</v>
       </c>
       <c r="B203" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C203" t="s">
         <v>419</v>
       </c>
       <c r="D203" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
     <row r="204" spans="1:4">
@@ -5083,13 +5131,13 @@
         <v>324</v>
       </c>
       <c r="B204" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C204" t="s">
         <v>419</v>
       </c>
       <c r="D204" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="205" spans="1:4">
@@ -5097,13 +5145,13 @@
         <v>324</v>
       </c>
       <c r="B205" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C205" t="s">
         <v>419</v>
       </c>
       <c r="D205" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
     </row>
     <row r="206" spans="1:4">
@@ -5111,13 +5159,13 @@
         <v>324</v>
       </c>
       <c r="B206" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="C206" t="s">
         <v>419</v>
       </c>
       <c r="D206" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
     <row r="207" spans="1:4">
@@ -5125,13 +5173,13 @@
         <v>324</v>
       </c>
       <c r="B207" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="C207" t="s">
         <v>419</v>
       </c>
       <c r="D207" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="208" spans="1:4">
@@ -5139,13 +5187,13 @@
         <v>324</v>
       </c>
       <c r="B208" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C208" t="s">
         <v>419</v>
       </c>
       <c r="D208" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
     </row>
     <row r="209" spans="1:4">
@@ -5153,13 +5201,13 @@
         <v>324</v>
       </c>
       <c r="B209" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C209" t="s">
         <v>419</v>
       </c>
       <c r="D209" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
     </row>
     <row r="210" spans="1:4">
@@ -5167,13 +5215,13 @@
         <v>324</v>
       </c>
       <c r="B210" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C210" t="s">
         <v>419</v>
       </c>
       <c r="D210" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="211" spans="1:4">
@@ -5181,69 +5229,69 @@
         <v>324</v>
       </c>
       <c r="B211" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="C211" t="s">
         <v>419</v>
       </c>
       <c r="D211" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="212" spans="1:4">
       <c r="A212" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B212" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="C212" t="s">
-        <v>443</v>
+        <v>419</v>
       </c>
       <c r="D212" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
     </row>
     <row r="213" spans="1:4">
       <c r="A213" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B213" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="C213" t="s">
-        <v>443</v>
+        <v>419</v>
       </c>
       <c r="D213" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
     </row>
     <row r="214" spans="1:4">
       <c r="A214" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B214" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="C214" t="s">
-        <v>443</v>
+        <v>419</v>
       </c>
       <c r="D214" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="215" spans="1:4">
       <c r="A215" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B215" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="C215" t="s">
-        <v>443</v>
+        <v>419</v>
       </c>
       <c r="D215" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
     </row>
     <row r="216" spans="1:4">
@@ -5251,13 +5299,13 @@
         <v>325</v>
       </c>
       <c r="B216" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C216" t="s">
         <v>443</v>
       </c>
       <c r="D216" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
     </row>
     <row r="217" spans="1:4">
@@ -5265,13 +5313,13 @@
         <v>325</v>
       </c>
       <c r="B217" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="C217" t="s">
         <v>443</v>
       </c>
       <c r="D217" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
     </row>
     <row r="218" spans="1:4">
@@ -5279,13 +5327,13 @@
         <v>325</v>
       </c>
       <c r="B218" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C218" t="s">
         <v>443</v>
       </c>
       <c r="D218" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
     </row>
     <row r="219" spans="1:4">
@@ -5293,13 +5341,13 @@
         <v>325</v>
       </c>
       <c r="B219" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="C219" t="s">
         <v>443</v>
       </c>
       <c r="D219" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
     </row>
     <row r="220" spans="1:4">
@@ -5307,13 +5355,13 @@
         <v>325</v>
       </c>
       <c r="B220" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="C220" t="s">
         <v>443</v>
       </c>
       <c r="D220" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
     </row>
     <row r="221" spans="1:4">
@@ -5321,13 +5369,13 @@
         <v>325</v>
       </c>
       <c r="B221" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C221" t="s">
         <v>443</v>
       </c>
       <c r="D221" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
     </row>
     <row r="222" spans="1:4">
@@ -5335,13 +5383,13 @@
         <v>325</v>
       </c>
       <c r="B222" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C222" t="s">
         <v>443</v>
       </c>
       <c r="D222" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
     </row>
     <row r="223" spans="1:4">
@@ -5349,13 +5397,13 @@
         <v>325</v>
       </c>
       <c r="B223" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C223" t="s">
         <v>443</v>
       </c>
       <c r="D223" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="224" spans="1:4">
@@ -5363,13 +5411,13 @@
         <v>325</v>
       </c>
       <c r="B224" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="C224" t="s">
         <v>443</v>
       </c>
       <c r="D224" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
     </row>
     <row r="225" spans="1:4">
@@ -5377,13 +5425,13 @@
         <v>325</v>
       </c>
       <c r="B225" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="C225" t="s">
         <v>443</v>
       </c>
       <c r="D225" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
     </row>
     <row r="226" spans="1:4">
@@ -5391,13 +5439,13 @@
         <v>325</v>
       </c>
       <c r="B226" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C226" t="s">
         <v>443</v>
       </c>
       <c r="D226" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="227" spans="1:4">
@@ -5405,13 +5453,13 @@
         <v>325</v>
       </c>
       <c r="B227" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C227" t="s">
         <v>443</v>
       </c>
       <c r="D227" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="228" spans="1:4">
@@ -5419,13 +5467,13 @@
         <v>325</v>
       </c>
       <c r="B228" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="C228" t="s">
         <v>443</v>
       </c>
       <c r="D228" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
     </row>
     <row r="229" spans="1:4">
@@ -5433,13 +5481,13 @@
         <v>325</v>
       </c>
       <c r="B229" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C229" t="s">
         <v>443</v>
       </c>
       <c r="D229" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
     </row>
     <row r="230" spans="1:4">
@@ -5447,13 +5495,13 @@
         <v>325</v>
       </c>
       <c r="B230" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C230" t="s">
         <v>443</v>
       </c>
       <c r="D230" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
     </row>
     <row r="231" spans="1:4">
@@ -5461,13 +5509,13 @@
         <v>325</v>
       </c>
       <c r="B231" t="s">
-        <v>462</v>
+        <v>341</v>
       </c>
       <c r="C231" t="s">
         <v>443</v>
       </c>
       <c r="D231" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
     </row>
     <row r="232" spans="1:4">
@@ -5475,13 +5523,13 @@
         <v>325</v>
       </c>
       <c r="B232" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C232" t="s">
         <v>443</v>
       </c>
       <c r="D232" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
     </row>
     <row r="233" spans="1:4">
@@ -5489,13 +5537,13 @@
         <v>325</v>
       </c>
       <c r="B233" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C233" t="s">
         <v>443</v>
       </c>
       <c r="D233" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
     </row>
     <row r="234" spans="1:4">
@@ -5503,13 +5551,13 @@
         <v>325</v>
       </c>
       <c r="B234" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C234" t="s">
         <v>443</v>
       </c>
       <c r="D234" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
     </row>
     <row r="235" spans="1:4">
@@ -5517,69 +5565,69 @@
         <v>325</v>
       </c>
       <c r="B235" t="s">
-        <v>348</v>
+        <v>462</v>
       </c>
       <c r="C235" t="s">
         <v>443</v>
       </c>
       <c r="D235" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="236" spans="1:4">
       <c r="A236" t="s">
-        <v>349</v>
+        <v>325</v>
       </c>
       <c r="B236" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="C236" t="s">
-        <v>469</v>
+        <v>443</v>
       </c>
       <c r="D236" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
     </row>
     <row r="237" spans="1:4">
       <c r="A237" t="s">
-        <v>349</v>
+        <v>325</v>
       </c>
       <c r="B237" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="C237" t="s">
-        <v>469</v>
+        <v>443</v>
       </c>
       <c r="D237" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
     </row>
     <row r="238" spans="1:4">
       <c r="A238" t="s">
-        <v>349</v>
+        <v>325</v>
       </c>
       <c r="B238" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="C238" t="s">
-        <v>469</v>
+        <v>443</v>
       </c>
       <c r="D238" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
     </row>
     <row r="239" spans="1:4">
       <c r="A239" t="s">
-        <v>349</v>
+        <v>325</v>
       </c>
       <c r="B239" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="C239" t="s">
-        <v>469</v>
+        <v>443</v>
       </c>
       <c r="D239" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
     </row>
     <row r="240" spans="1:4">
@@ -5587,13 +5635,13 @@
         <v>349</v>
       </c>
       <c r="B240" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="C240" t="s">
         <v>469</v>
       </c>
       <c r="D240" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
     </row>
     <row r="241" spans="1:4">
@@ -5601,13 +5649,13 @@
         <v>349</v>
       </c>
       <c r="B241" t="s">
-        <v>509</v>
+        <v>351</v>
       </c>
       <c r="C241" t="s">
         <v>469</v>
       </c>
       <c r="D241" t="s">
-        <v>510</v>
+        <v>470</v>
       </c>
     </row>
     <row r="242" spans="1:4">
@@ -5615,13 +5663,13 @@
         <v>349</v>
       </c>
       <c r="B242" t="s">
-        <v>512</v>
+        <v>352</v>
       </c>
       <c r="C242" t="s">
         <v>469</v>
       </c>
       <c r="D242" t="s">
-        <v>514</v>
+        <v>471</v>
       </c>
     </row>
     <row r="243" spans="1:4">
@@ -5629,13 +5677,13 @@
         <v>349</v>
       </c>
       <c r="B243" t="s">
-        <v>513</v>
+        <v>353</v>
       </c>
       <c r="C243" t="s">
         <v>469</v>
       </c>
       <c r="D243" t="s">
-        <v>515</v>
+        <v>472</v>
       </c>
     </row>
     <row r="244" spans="1:4">
@@ -5643,13 +5691,13 @@
         <v>349</v>
       </c>
       <c r="B244" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C244" t="s">
         <v>469</v>
       </c>
       <c r="D244" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="245" spans="1:4">
@@ -5657,13 +5705,13 @@
         <v>349</v>
       </c>
       <c r="B245" t="s">
-        <v>356</v>
+        <v>509</v>
       </c>
       <c r="C245" t="s">
         <v>469</v>
       </c>
       <c r="D245" t="s">
-        <v>475</v>
+        <v>510</v>
       </c>
     </row>
     <row r="246" spans="1:4">
@@ -5671,13 +5719,13 @@
         <v>349</v>
       </c>
       <c r="B246" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="C246" t="s">
         <v>469</v>
       </c>
       <c r="D246" t="s">
-        <v>241</v>
+        <v>514</v>
       </c>
     </row>
     <row r="247" spans="1:4">
@@ -5685,13 +5733,13 @@
         <v>349</v>
       </c>
       <c r="B247" t="s">
-        <v>357</v>
+        <v>513</v>
       </c>
       <c r="C247" t="s">
         <v>469</v>
       </c>
       <c r="D247" t="s">
-        <v>476</v>
+        <v>515</v>
       </c>
     </row>
     <row r="248" spans="1:4">
@@ -5699,13 +5747,13 @@
         <v>349</v>
       </c>
       <c r="B248" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C248" t="s">
         <v>469</v>
       </c>
       <c r="D248" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
     </row>
     <row r="249" spans="1:4">
@@ -5713,13 +5761,13 @@
         <v>349</v>
       </c>
       <c r="B249" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C249" t="s">
         <v>469</v>
       </c>
       <c r="D249" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="250" spans="1:4">
@@ -5727,13 +5775,13 @@
         <v>349</v>
       </c>
       <c r="B250" t="s">
-        <v>360</v>
+        <v>511</v>
       </c>
       <c r="C250" t="s">
         <v>469</v>
       </c>
       <c r="D250" t="s">
-        <v>479</v>
+        <v>241</v>
       </c>
     </row>
     <row r="251" spans="1:4">
@@ -5741,13 +5789,13 @@
         <v>349</v>
       </c>
       <c r="B251" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="C251" t="s">
         <v>469</v>
       </c>
       <c r="D251" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
     </row>
     <row r="252" spans="1:4">
@@ -5755,13 +5803,13 @@
         <v>349</v>
       </c>
       <c r="B252" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="C252" t="s">
         <v>469</v>
       </c>
       <c r="D252" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
     </row>
     <row r="253" spans="1:4">
@@ -5769,13 +5817,13 @@
         <v>349</v>
       </c>
       <c r="B253" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="C253" t="s">
         <v>469</v>
       </c>
       <c r="D253" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
     </row>
     <row r="254" spans="1:4">
@@ -5783,13 +5831,13 @@
         <v>349</v>
       </c>
       <c r="B254" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="C254" t="s">
         <v>469</v>
       </c>
       <c r="D254" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
     </row>
     <row r="255" spans="1:4">
@@ -5797,13 +5845,13 @@
         <v>349</v>
       </c>
       <c r="B255" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="C255" t="s">
         <v>469</v>
       </c>
       <c r="D255" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
     </row>
     <row r="256" spans="1:4">
@@ -5811,13 +5859,13 @@
         <v>349</v>
       </c>
       <c r="B256" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="C256" t="s">
         <v>469</v>
       </c>
       <c r="D256" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
     </row>
     <row r="257" spans="1:4">
@@ -5825,13 +5873,13 @@
         <v>349</v>
       </c>
       <c r="B257" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="C257" t="s">
         <v>469</v>
       </c>
       <c r="D257" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
     </row>
     <row r="258" spans="1:4">
@@ -5839,13 +5887,13 @@
         <v>349</v>
       </c>
       <c r="B258" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C258" t="s">
         <v>469</v>
       </c>
       <c r="D258" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
     </row>
     <row r="259" spans="1:4">
@@ -5853,13 +5901,13 @@
         <v>349</v>
       </c>
       <c r="B259" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="C259" t="s">
         <v>469</v>
       </c>
       <c r="D259" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="260" spans="1:4">
@@ -5867,41 +5915,125 @@
         <v>349</v>
       </c>
       <c r="B260" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="C260" t="s">
         <v>469</v>
       </c>
       <c r="D260" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
     </row>
     <row r="261" spans="1:4">
       <c r="A261" t="s">
-        <v>371</v>
+        <v>349</v>
       </c>
       <c r="B261" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="C261" t="s">
-        <v>490</v>
+        <v>469</v>
       </c>
       <c r="D261" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
     </row>
     <row r="262" spans="1:4">
       <c r="A262" t="s">
+        <v>349</v>
+      </c>
+      <c r="B262" t="s">
+        <v>368</v>
+      </c>
+      <c r="C262" t="s">
+        <v>469</v>
+      </c>
+      <c r="D262" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4">
+      <c r="A263" t="s">
+        <v>349</v>
+      </c>
+      <c r="B263" t="s">
+        <v>369</v>
+      </c>
+      <c r="C263" t="s">
+        <v>469</v>
+      </c>
+      <c r="D263" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4">
+      <c r="A264" t="s">
+        <v>349</v>
+      </c>
+      <c r="B264" t="s">
+        <v>370</v>
+      </c>
+      <c r="C264" t="s">
+        <v>469</v>
+      </c>
+      <c r="D264" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4">
+      <c r="A265" t="s">
         <v>371</v>
       </c>
-      <c r="B262" t="s">
+      <c r="B265" t="s">
+        <v>372</v>
+      </c>
+      <c r="C265" t="s">
+        <v>490</v>
+      </c>
+      <c r="D265" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4">
+      <c r="A266" t="s">
+        <v>371</v>
+      </c>
+      <c r="B266" t="s">
         <v>373</v>
       </c>
-      <c r="C262" t="s">
+      <c r="C266" t="s">
         <v>490</v>
       </c>
-      <c r="D262" t="s">
+      <c r="D266" t="s">
         <v>492</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4">
+      <c r="A267" t="s">
+        <v>371</v>
+      </c>
+      <c r="B267" t="s">
+        <v>524</v>
+      </c>
+      <c r="C267" t="s">
+        <v>490</v>
+      </c>
+      <c r="D267" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4">
+      <c r="A268" t="s">
+        <v>371</v>
+      </c>
+      <c r="B268" t="s">
+        <v>525</v>
+      </c>
+      <c r="C268" t="s">
+        <v>490</v>
+      </c>
+      <c r="D268" t="s">
+        <v>527</v>
       </c>
     </row>
   </sheetData>

</xml_diff>